<commit_message>
tdf#94231 OOXML Import: Fix disappeared Hatch Background Color
With adding the PROP_FillBackground property to spnCommonPropIds and
spnFilledPropIds the hatch background color imported correctly,
an will not disappear.

Change-Id: I56745179236d2912a2d5c8585098e54acc4e3062
Reviewed-on: https://gerrit.libreoffice.org/63069
Tested-by: Jenkins
Reviewed-by: Markus Mohrhard <markus.mohrhard@googlemail.com>
</commit_message>
<xml_diff>
--- a/chart2/qa/extras/data/xlsx/chart-hatch-fill.xlsx
+++ b/chart2/qa/extras/data/xlsx/chart-hatch-fill.xlsx
@@ -188,7 +188,7 @@
                   <a:schemeClr val="accent6"/>
                 </a:fgClr>
                 <a:bgClr>
-                  <a:schemeClr val="bg1"/>
+                  <a:srgbClr val="00B050"/>
                 </a:bgClr>
               </a:pattFill>
             </c:spPr>
@@ -644,7 +644,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>